<commit_message>
1. 슬로우 모션 테스트 ( O, P 키 ) 2. Render State 수정 ( 메쉬 - BACKUI - 플레이어 순서 ) 3. BackUI 테스트 객체 생성
</commit_message>
<xml_diff>
--- a/해야 할 일.xlsx
+++ b/해야 할 일.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{310B3893-AE1D-4FB7-B3C6-E511E2C1695B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="68">
   <si>
     <t>No.</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -263,13 +262,41 @@
   </si>
   <si>
     <t>Static</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>순간이동</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>툴</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>대부분</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이펙트</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>슬로모션</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>자동문</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>게임밖으로</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -312,7 +339,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -518,11 +545,59 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -541,6 +616,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -820,11 +899,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -832,8 +911,8 @@
     <col min="2" max="2" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>0</v>
       </c>
@@ -847,7 +926,7 @@
       <c r="I2" s="2"/>
       <c r="J2" s="3"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="11">
         <v>1</v>
       </c>
@@ -860,14 +939,18 @@
       <c r="D3" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
+      <c r="E3" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F3" s="15" t="s">
+        <v>25</v>
+      </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="4"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="11">
         <v>2</v>
       </c>
@@ -891,7 +974,7 @@
       <c r="I4" s="1"/>
       <c r="J4" s="4"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="11">
         <v>3</v>
       </c>
@@ -911,7 +994,7 @@
       <c r="I5" s="1"/>
       <c r="J5" s="4"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="11">
         <v>4</v>
       </c>
@@ -935,7 +1018,7 @@
       <c r="I6" s="1"/>
       <c r="J6" s="4"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="11">
         <v>5</v>
       </c>
@@ -963,7 +1046,7 @@
       <c r="I7" s="1"/>
       <c r="J7" s="4"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="11">
         <v>6</v>
       </c>
@@ -987,7 +1070,7 @@
       <c r="I8" s="1"/>
       <c r="J8" s="4"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="11">
         <v>7</v>
       </c>
@@ -1019,7 +1102,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="11">
         <v>8</v>
       </c>
@@ -1043,7 +1126,7 @@
       <c r="I10" s="1"/>
       <c r="J10" s="4"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="11">
         <v>9</v>
       </c>
@@ -1065,13 +1148,23 @@
       <c r="G11" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="H11" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="I11" s="1"/>
-      <c r="J11" s="4"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="H11" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="J11" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="K11" t="s">
+        <v>66</v>
+      </c>
+      <c r="L11" s="15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="11">
         <v>10</v>
       </c>
@@ -1090,8 +1183,14 @@
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="4"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K12" t="s">
+        <v>67</v>
+      </c>
+      <c r="L12" s="15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="11">
         <v>11</v>
       </c>
@@ -1115,7 +1214,7 @@
       <c r="I13" s="1"/>
       <c r="J13" s="4"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="11">
         <v>12</v>
       </c>
@@ -1143,7 +1242,7 @@
       <c r="I14" s="1"/>
       <c r="J14" s="4"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="11">
         <v>13</v>
       </c>
@@ -1167,7 +1266,7 @@
       <c r="I15" s="1"/>
       <c r="J15" s="4"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="11">
         <v>14</v>
       </c>
@@ -1307,29 +1406,53 @@
       <c r="I20" s="1"/>
       <c r="J20" s="4"/>
     </row>
-    <row r="21" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="11">
         <v>19</v>
       </c>
-      <c r="B21" s="14" t="s">
+      <c r="B21" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="C21" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="D21" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="E21" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="F21" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="G21" s="20"/>
+      <c r="H21" s="20"/>
+      <c r="I21" s="20"/>
+      <c r="J21" s="21"/>
+    </row>
+    <row r="22" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="11">
+        <v>20</v>
+      </c>
+      <c r="B22" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="C21" s="9" t="s">
+      <c r="C22" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="D21" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="E21" s="5" t="s">
+      <c r="D22" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E22" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="F21" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="G21" s="5"/>
-      <c r="H21" s="5"/>
-      <c r="I21" s="5"/>
-      <c r="J21" s="6"/>
+      <c r="F22" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="5"/>
+      <c r="J22" s="6"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>